<commit_message>
Adjust for cuts & Semi files
</commit_message>
<xml_diff>
--- a/Fall 2023/Microwave Engineering/Project/Data.xlsx
+++ b/Fall 2023/Microwave Engineering/Project/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Fall 2023\Microwave Engineering\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6172E074-4FFF-46DC-96EC-247B66317112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A1D2CE-10CC-47E4-A222-3D04E413D76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,8 +196,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,90 +677,54 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$31</c:f>
+              <c:f>Sheet1!$D$20:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>0.86250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.92500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>1.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.92247999999999997</c:v>
+                  <c:v>1.1125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.92842999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.93030999999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.93208000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.93269999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.3</c:v>
+                  <c:v>1.2375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$31</c:f>
+              <c:f>Sheet1!$G$20:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.39621127539202528</c:v>
+                  <c:v>6.5134483244196364E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18746697962362682</c:v>
+                  <c:v>5.8409535922327491E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10266175232179583</c:v>
+                  <c:v>5.4341719062644095E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1404923096693879E-2</c:v>
+                  <c:v>4.9346249471626705E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8073064912315238E-2</c:v>
+                  <c:v>4.0330892598186549E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.3287260258119399E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.4734433333850594E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.0885152681025713E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.3213793006457089E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.3347022919493475E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.7795619205841064E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.0520112970485453E-2</c:v>
+                  <c:v>3.9400062434284136E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3382,8 +3346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C03D3BA-7F5A-483D-B888-8A7D711FA949}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="V55" sqref="V55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3527,14 +3491,14 @@
         <v>3.92</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:M18" si="0">K9-90</f>
+        <f t="shared" ref="M9:M15" si="0">K9-90</f>
         <v>-97.44</v>
       </c>
       <c r="N9" s="5">
         <v>4.0910000000000002</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9:O18" si="1">K9+90</f>
+        <f t="shared" ref="O9:O15" si="1">K9+90</f>
         <v>82.56</v>
       </c>
       <c r="P9">
@@ -3556,14 +3520,14 @@
         <v>3.9119999999999999</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10" si="2">K10-90</f>
+        <f t="shared" si="0"/>
         <v>-98.05</v>
       </c>
       <c r="N10" s="4">
         <v>4.1219999999999999</v>
       </c>
       <c r="O10">
-        <f t="shared" ref="O10" si="3">K10+90</f>
+        <f t="shared" si="1"/>
         <v>81.95</v>
       </c>
       <c r="P10">
@@ -3588,18 +3552,18 @@
         <v>3.907</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:M15" si="4">K11-90</f>
+        <f t="shared" si="0"/>
         <v>-96.67</v>
       </c>
       <c r="N11">
         <v>4.149</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O15" si="5">K11+90</f>
+        <f t="shared" si="1"/>
         <v>83.33</v>
       </c>
       <c r="P11">
-        <f t="shared" ref="P11:P15" si="6">ABS(J11/(N11-L11))</f>
+        <f>ABS(J11/(N11-L11))</f>
         <v>16.644628099173552</v>
       </c>
     </row>
@@ -3614,31 +3578,31 @@
         <v>14</v>
       </c>
       <c r="I12">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="J12">
-        <v>4.0179999999999998</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="K12">
-        <v>-8.0500000000000007</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L12">
-        <v>4.1219999999999999</v>
+        <v>3.871</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
-        <v>-98.05</v>
+        <f t="shared" si="0"/>
+        <v>-89.93</v>
       </c>
       <c r="N12">
-        <v>5.9119999999999999</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
-        <v>81.95</v>
+        <f t="shared" si="1"/>
+        <v>90.07</v>
       </c>
       <c r="P12">
-        <f t="shared" si="6"/>
-        <v>2.2446927374301673</v>
+        <f>ABS(J12/(N12-L12))</f>
+        <v>14.379928315412167</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -3649,31 +3613,31 @@
         <v>3.55</v>
       </c>
       <c r="I13">
-        <v>2.1</v>
+        <v>2.8521000000000001</v>
       </c>
       <c r="J13">
-        <v>4.0179999999999998</v>
+        <v>4.0229999999999997</v>
       </c>
       <c r="K13">
-        <v>-8.0500000000000007</v>
+        <v>-3.44</v>
       </c>
       <c r="L13">
-        <v>4.1219999999999999</v>
+        <v>3.8759999999999999</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
-        <v>-98.05</v>
+        <f t="shared" si="0"/>
+        <v>-93.44</v>
       </c>
       <c r="N13">
-        <v>6.9119999999999999</v>
+        <v>4.1719999999999997</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
-        <v>81.95</v>
+        <f t="shared" si="1"/>
+        <v>86.56</v>
       </c>
       <c r="P13">
-        <f t="shared" si="6"/>
-        <v>1.4401433691756271</v>
+        <f>ABS(J13/(N13-L13))</f>
+        <v>13.591216216216223</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -3687,31 +3651,31 @@
         <v>12</v>
       </c>
       <c r="I14">
-        <v>2.1</v>
+        <v>2.86</v>
       </c>
       <c r="J14">
         <v>4.0179999999999998</v>
       </c>
       <c r="K14">
-        <v>-8.0500000000000007</v>
+        <v>-0.11</v>
       </c>
       <c r="L14">
-        <v>4.1219999999999999</v>
+        <v>3.8679999999999999</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
-        <v>-98.05</v>
+        <f t="shared" si="0"/>
+        <v>-90.11</v>
       </c>
       <c r="N14">
-        <v>7.9119999999999999</v>
+        <v>4.1660000000000004</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
-        <v>81.95</v>
+        <f t="shared" si="1"/>
+        <v>89.89</v>
       </c>
       <c r="P14">
-        <f t="shared" si="6"/>
-        <v>1.0601583113456463</v>
+        <f>ABS(J14/(N14-L14))</f>
+        <v>13.483221476510044</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -3725,31 +3689,31 @@
         <v>12</v>
       </c>
       <c r="I15">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="J15">
-        <v>4.0179999999999998</v>
+        <v>4.0229999999999997</v>
       </c>
       <c r="K15">
-        <v>-8.0500000000000007</v>
+        <v>0.24</v>
       </c>
       <c r="L15">
-        <v>4.1219999999999999</v>
+        <v>3.863</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
-        <v>-98.05</v>
+        <f t="shared" si="0"/>
+        <v>-89.76</v>
       </c>
       <c r="N15">
-        <v>8.9120000000000008</v>
+        <v>4.1820000000000004</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
-        <v>81.95</v>
+        <f t="shared" si="1"/>
+        <v>90.24</v>
       </c>
       <c r="P15">
-        <f t="shared" si="6"/>
-        <v>0.83883089770354891</v>
+        <f>ABS(J15/(N15-L15))</f>
+        <v>12.611285266457664</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -3799,17 +3763,17 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E20" s="2">
-        <v>2.6714000000000002</v>
+        <v>3.7669999999999999</v>
       </c>
       <c r="F20" s="2">
-        <v>4.0622999999999996</v>
+        <v>4.0209000000000001</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" ref="G20:G31" si="7">(F20^2-E20^2)/(F20^2+E20^2)</f>
-        <v>0.39621127539202528</v>
+        <f t="shared" ref="G20" si="2">(F20^2-E20^2)/(F20^2+E20^2)</f>
+        <v>6.5134483244196364E-2</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
@@ -3820,17 +3784,17 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
-        <v>0.25</v>
+        <v>0.86250000000000004</v>
       </c>
       <c r="E21" s="2">
-        <v>3.09</v>
+        <v>3.8426</v>
       </c>
       <c r="F21" s="2">
-        <v>3.7355</v>
+        <v>4.0739999999999998</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="7"/>
-        <v>0.18746697962362682</v>
+        <f>(F21^2-E21^2)/(F21^2+E21^2)</f>
+        <v>5.8409535922327491E-2</v>
       </c>
       <c r="I21">
         <v>20</v>
@@ -3841,17 +3805,17 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
-        <v>0.5</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="E22" s="2">
-        <v>3.7246999999999999</v>
+        <v>3.8174000000000001</v>
       </c>
       <c r="F22" s="2">
-        <v>4.1288999999999998</v>
+        <v>4.0308000000000002</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="7"/>
-        <v>0.10266175232179583</v>
+        <f t="shared" ref="G22" si="3">(F22^2-E22^2)/(F22^2+E22^2)</f>
+        <v>5.4341719062644095E-2</v>
       </c>
       <c r="I22">
         <v>21.6173</v>
@@ -3862,17 +3826,17 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
-        <v>0.75</v>
+        <v>1.05</v>
       </c>
       <c r="E23" s="2">
-        <v>3.5373999999999999</v>
+        <v>3.7688000000000001</v>
       </c>
       <c r="F23" s="2">
-        <v>3.8380999999999998</v>
+        <v>3.9596</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="7"/>
-        <v>8.1404923096693879E-2</v>
+        <f t="shared" ref="G23:G30" si="4">(F23^2-E23^2)/(F23^2+E23^2)</f>
+        <v>4.9346249471626705E-2</v>
       </c>
       <c r="I23">
         <v>21.6812</v>
@@ -3882,18 +3846,18 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="2">
-        <v>0.92247999999999997</v>
+      <c r="D24" s="3">
+        <v>1.1125</v>
       </c>
       <c r="E24" s="2">
-        <v>3.7904</v>
+        <v>3.8029999999999999</v>
       </c>
       <c r="F24" s="2">
-        <v>4.0172999999999996</v>
+        <v>3.9596</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="7"/>
-        <v>5.8073064912315238E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.0330892598186549E-2</v>
       </c>
       <c r="I24">
         <v>21.754000000000001</v>
@@ -3904,17 +3868,17 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D25" s="3">
-        <v>0.92842999999999998</v>
+        <v>1.2375</v>
       </c>
       <c r="E25" s="2">
-        <v>3.7418</v>
+        <v>3.7157</v>
       </c>
       <c r="F25" s="2">
-        <v>3.9866000000000001</v>
+        <v>3.8651</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="7"/>
-        <v>6.3287260258119399E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.9400062434284136E-2</v>
       </c>
       <c r="I25">
         <v>21.85</v>
@@ -3924,18 +3888,18 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="3">
-        <v>0.93030999999999997</v>
+      <c r="D26" s="2">
+        <v>0.82869000000000004</v>
       </c>
       <c r="E26" s="2">
-        <v>3.7507999999999999</v>
+        <v>3.7553000000000001</v>
       </c>
       <c r="F26" s="2">
-        <v>4.0019999999999998</v>
+        <v>3.9965000000000002</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="7"/>
-        <v>6.4734433333850594E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.2170516373354932E-2</v>
       </c>
       <c r="I26">
         <v>22</v>
@@ -3946,17 +3910,17 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
-        <v>0.93208000000000002</v>
+        <v>1.0636000000000001</v>
       </c>
       <c r="E27" s="2">
-        <v>3.6941000000000002</v>
+        <v>3.7652000000000001</v>
       </c>
       <c r="F27" s="2">
-        <v>3.9262999999999999</v>
+        <v>3.9731000000000001</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="7"/>
-        <v>6.0885152681025713E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.369397559672634E-2</v>
       </c>
       <c r="I27">
         <v>24</v>
@@ -3968,17 +3932,17 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="3">
-        <v>0.93269999999999997</v>
+        <v>1.0742</v>
       </c>
       <c r="E28" s="2">
-        <v>3.7463000000000002</v>
+        <v>3.2286999999999999</v>
       </c>
       <c r="F28" s="2">
-        <v>3.9910999999999999</v>
+        <v>3.4266999999999999</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="7"/>
-        <v>6.3213793006457089E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.9447939814080045E-2</v>
       </c>
       <c r="I28">
         <v>26</v>
@@ -3990,17 +3954,17 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="2">
-        <v>1</v>
+        <v>1.0722</v>
       </c>
       <c r="E29" s="2">
-        <v>3.7904</v>
+        <v>3.8012000000000001</v>
       </c>
       <c r="F29" s="2">
-        <v>3.9983</v>
+        <v>3.9883999999999999</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="7"/>
-        <v>5.3347022919493475E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.8036342582282926E-2</v>
       </c>
       <c r="I29">
         <v>28</v>
@@ -4011,33 +3975,24 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
-        <v>1.25</v>
+        <v>1.071</v>
       </c>
       <c r="E30" s="2">
-        <v>3.7841</v>
+        <v>3.8174000000000001</v>
       </c>
       <c r="F30" s="2">
-        <v>3.9695</v>
+        <v>3.9929000000000001</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="7"/>
-        <v>4.7795619205841064E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.4917975500880614E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="E31" s="2">
-        <v>3.6760999999999999</v>
-      </c>
-      <c r="F31" s="2">
-        <v>3.8281999999999998</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" si="7"/>
-        <v>4.0520112970485453E-2</v>
-      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D32" s="2"/>

</xml_diff>

<commit_message>
Redo project with bigger gap (sims inc)
</commit_message>
<xml_diff>
--- a/Fall 2023/Microwave Engineering/Project/Data.xlsx
+++ b/Fall 2023/Microwave Engineering/Project/Data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Fall 2023\Microwave Engineering\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A1D2CE-10CC-47E4-A222-3D04E413D76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DBF999-E5DF-4CE8-9253-6DCCA6C8C4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Resonator Synthesis" sheetId="2" r:id="rId2"/>
+    <sheet name="Qext Synthesis" sheetId="3" r:id="rId3"/>
+    <sheet name="K Synthesis" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>g</t>
   </si>
@@ -128,12 +130,33 @@
   <si>
     <t>Spacing</t>
   </si>
+  <si>
+    <t>Simulation Pass 1</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>Leg</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>Optimal values</t>
+  </si>
+  <si>
+    <t>With gap = 0.5mm</t>
+  </si>
+  <si>
+    <t>Gap=0.42 mm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +170,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +192,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -181,11 +218,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -198,11 +279,269 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3003,6 +3342,197 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>588038</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>122690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A graph of a graph showing a variety of colors&#10;&#10;Description automatically generated with medium confidence">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5C81F06-5578-0FCC-7167-62F793A3EEB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="190500"/>
+          <a:ext cx="20095238" cy="9076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>359227</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>122238</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>132117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="A graph with many colored dots&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE4E6EFF-9A27-E188-934D-7806C7C8BD79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7674427" y="9667875"/>
+          <a:ext cx="4639811" cy="3608742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>473738</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>120135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A graph of different colored lines&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3614B09E-2E08-C216-87BE-B77C4634AB69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9315450" y="0"/>
+          <a:ext cx="17980688" cy="8121135"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>122773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>530887</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>186575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A graph of different colored lines&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368F8903-CFC7-F222-F6A2-4532F441D378}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="503773"/>
+          <a:ext cx="8998612" cy="4064302"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B62A11DF-F8CB-4A8E-8671-BD80D0959120}" name="Table1" displayName="Table1" ref="I8:P18" totalsRowShown="0">
   <autoFilter ref="I8:P18" xr:uid="{B62A11DF-F8CB-4A8E-8671-BD80D0959120}"/>
@@ -3030,17 +3560,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A5BE6DB7-518C-4D5D-BCFA-A195FB212AA8}" name="Table2" displayName="Table2" ref="D19:G42" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A5BE6DB7-518C-4D5D-BCFA-A195FB212AA8}" name="Table2" displayName="Table2" ref="D19:G42" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="D19:G42" xr:uid="{A5BE6DB7-518C-4D5D-BCFA-A195FB212AA8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D20:G42">
     <sortCondition ref="D19:D42"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F1AFA0AC-5393-43F3-AD3B-AF9A03A0CE6A}" name="Spacing" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C59E817E-B8E5-4C50-B578-20EF163F5DB5}" name="fm" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{37E70FEC-B763-412C-93A8-62B6A42E1A29}" name="fe" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{468476DE-B358-4BA4-BA6C-2D2289057D38}" name="k12" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{F1AFA0AC-5393-43F3-AD3B-AF9A03A0CE6A}" name="Spacing" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{C59E817E-B8E5-4C50-B578-20EF163F5DB5}" name="fm" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{37E70FEC-B763-412C-93A8-62B6A42E1A29}" name="fe" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{468476DE-B358-4BA4-BA6C-2D2289057D38}" name="k12" dataDxfId="9">
       <calculatedColumnFormula>(F20^2-E20^2)/(F20^2+E20^2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{55FEDA29-AB2B-4C70-9B9B-75AB59D53983}" name="Table3" displayName="Table3" ref="B4:E12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="B4:E12" xr:uid="{55FEDA29-AB2B-4C70-9B9B-75AB59D53983}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E11">
+    <sortCondition ref="B4:B11"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F3E3B381-05AC-45A9-93A3-F0AB3D687519}" name="Spacing" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{7B3BD53E-1547-43C1-B438-211461B91917}" name="fm" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3365EFB3-39BC-43B8-9F1A-AE6C8980A1F9}" name="fe" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{3B3FEAE3-E71D-4113-B448-E8C1D7A50362}" name="kij" dataDxfId="2">
+      <calculatedColumnFormula>(D5^2-C5^2)/(D5^2+C5^2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3346,8 +3894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C03D3BA-7F5A-483D-B888-8A7D711FA949}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="V55" sqref="V55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4137,12 +4685,923 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBBA627-5AD6-4DBF-B35D-AA71A4FC1916}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.15</v>
+      </c>
+      <c r="C4">
+        <v>0.34</v>
+      </c>
+      <c r="D4">
+        <v>4.5319000000000003</v>
+      </c>
+      <c r="E4">
+        <v>-37.545200000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.15</v>
+      </c>
+      <c r="C5">
+        <v>0.36</v>
+      </c>
+      <c r="D5">
+        <v>4.2628000000000004</v>
+      </c>
+      <c r="E5">
+        <v>-36.411299999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.15</v>
+      </c>
+      <c r="C6">
+        <v>0.38</v>
+      </c>
+      <c r="D6">
+        <v>4.0861000000000001</v>
+      </c>
+      <c r="E6">
+        <v>-37.922699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.15</v>
+      </c>
+      <c r="C7">
+        <v>0.4</v>
+      </c>
+      <c r="D7">
+        <v>3.9015</v>
+      </c>
+      <c r="E7">
+        <v>-36.195099999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+      <c r="C8">
+        <v>0.34</v>
+      </c>
+      <c r="D8">
+        <v>3.7915000000000001</v>
+      </c>
+      <c r="E8">
+        <v>-44.752400000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+      <c r="C9">
+        <v>0.36</v>
+      </c>
+      <c r="D9">
+        <v>3.62</v>
+      </c>
+      <c r="E9">
+        <v>-41.591500000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>0.38</v>
+      </c>
+      <c r="D10">
+        <v>3.4733000000000001</v>
+      </c>
+      <c r="E10">
+        <v>-44.286099999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11">
+        <v>0.4</v>
+      </c>
+      <c r="D11">
+        <v>3.3182</v>
+      </c>
+      <c r="E11">
+        <v>-48.4041</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.4</v>
+      </c>
+      <c r="D12">
+        <v>3.1177999999999999</v>
+      </c>
+      <c r="E12">
+        <v>-45.857100000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.38</v>
+      </c>
+      <c r="D13">
+        <v>3.2867000000000002</v>
+      </c>
+      <c r="E13">
+        <v>-45.0929</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C14">
+        <v>0.36</v>
+      </c>
+      <c r="D14">
+        <v>3.4033000000000002</v>
+      </c>
+      <c r="E14">
+        <v>-51.444400000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.34</v>
+      </c>
+      <c r="D15">
+        <v>3.5794000000000001</v>
+      </c>
+      <c r="E15">
+        <v>-48.075200000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.32</v>
+      </c>
+      <c r="D16">
+        <v>3.7574000000000001</v>
+      </c>
+      <c r="E16">
+        <v>-45.230499999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0.25</v>
+      </c>
+      <c r="C17">
+        <v>0.4</v>
+      </c>
+      <c r="D17">
+        <v>2.9941</v>
+      </c>
+      <c r="E17">
+        <v>-49.138199999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0.25</v>
+      </c>
+      <c r="C18">
+        <v>0.38</v>
+      </c>
+      <c r="D18">
+        <v>3.1217999999999999</v>
+      </c>
+      <c r="E18">
+        <v>-49.728400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.25</v>
+      </c>
+      <c r="C19">
+        <v>0.36</v>
+      </c>
+      <c r="D19">
+        <v>3.2475000000000001</v>
+      </c>
+      <c r="E19">
+        <v>-47.821100000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0.25</v>
+      </c>
+      <c r="C20">
+        <v>0.34</v>
+      </c>
+      <c r="D20">
+        <v>3.3378000000000001</v>
+      </c>
+      <c r="E20">
+        <v>-57.676900000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.25</v>
+      </c>
+      <c r="C21">
+        <v>0.32</v>
+      </c>
+      <c r="D21">
+        <v>3.548</v>
+      </c>
+      <c r="E21">
+        <v>-53.576999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0.25</v>
+      </c>
+      <c r="C22">
+        <v>0.3</v>
+      </c>
+      <c r="D22">
+        <v>3.7149000000000001</v>
+      </c>
+      <c r="E22">
+        <v>-42.750900000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.25</v>
+      </c>
+      <c r="C23">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D23">
+        <v>3.91</v>
+      </c>
+      <c r="E23">
+        <v>-41.195099999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C28">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="D28">
+        <v>3.6015999999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257E1EC6-69F7-487F-B9CB-70A63808C60E}">
+  <dimension ref="B3:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4.141</v>
+      </c>
+      <c r="D5" s="7">
+        <v>110.05</v>
+      </c>
+      <c r="E5" s="7">
+        <v>4.0439999999999996</v>
+      </c>
+      <c r="F5" s="7">
+        <f>D5-90</f>
+        <v>20.049999999999997</v>
+      </c>
+      <c r="G5" s="7">
+        <v>4.2779999999999996</v>
+      </c>
+      <c r="H5" s="7">
+        <f>F5-180</f>
+        <v>-159.94999999999999</v>
+      </c>
+      <c r="I5" s="8">
+        <f>ABS(C5/(E5-G5))</f>
+        <v>17.696581196581199</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4.2110000000000003</v>
+      </c>
+      <c r="D6" s="7">
+        <v>117.11</v>
+      </c>
+      <c r="E6" s="7">
+        <v>4.0830000000000002</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" ref="F6:F10" si="0">D6-90</f>
+        <v>27.11</v>
+      </c>
+      <c r="G6" s="7">
+        <v>4.4109999999999996</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" ref="H6:H10" si="1">F6-180</f>
+        <v>-152.88999999999999</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" ref="I6:I10" si="2">ABS(C6/(E6-G6))</f>
+        <v>12.838414634146366</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4.202</v>
+      </c>
+      <c r="D7" s="7">
+        <v>123.37</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4.0570000000000004</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="0"/>
+        <v>33.370000000000005</v>
+      </c>
+      <c r="G7" s="7">
+        <v>4.4509999999999996</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="1"/>
+        <v>-146.63</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="2"/>
+        <v>10.66497461928936</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4.157</v>
+      </c>
+      <c r="D8" s="7">
+        <v>127.23</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4.0019999999999998</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="0"/>
+        <v>37.230000000000004</v>
+      </c>
+      <c r="G8" s="7">
+        <v>4.4509999999999996</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
+        <v>-142.76999999999998</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="2"/>
+        <v>9.2583518930957709</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4.1479999999999997</v>
+      </c>
+      <c r="D9" s="7">
+        <v>129.68</v>
+      </c>
+      <c r="E9" s="7">
+        <v>3.9750000000000001</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
+        <v>39.680000000000007</v>
+      </c>
+      <c r="G9" s="7">
+        <v>4.4909999999999997</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="1"/>
+        <v>-140.32</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="2"/>
+        <v>8.038759689922486</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4.1059999999999999</v>
+      </c>
+      <c r="D10" s="7">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3.9489999999999998</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
+        <v>48.699999999999989</v>
+      </c>
+      <c r="G10" s="7">
+        <v>4.4889999999999999</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="1"/>
+        <v>-131.30000000000001</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" si="2"/>
+        <v>7.6037037037037027</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4.17</v>
+      </c>
+      <c r="D11" s="7">
+        <v>116.13</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4.0490000000000004</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" ref="F11" si="3">D11-90</f>
+        <v>26.129999999999995</v>
+      </c>
+      <c r="G11" s="7">
+        <v>4.3540000000000001</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" ref="H11" si="4">F11-180</f>
+        <v>-153.87</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" ref="I11" si="5">ABS(C11/(E11-G11))</f>
+        <v>13.672131147540997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4.1950000000000003</v>
+      </c>
+      <c r="D12" s="7">
+        <v>115.96</v>
+      </c>
+      <c r="E12" s="7">
+        <v>4.07</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" ref="F12" si="6">D12-90</f>
+        <v>25.959999999999994</v>
+      </c>
+      <c r="G12" s="7">
+        <v>4.3860000000000001</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" ref="H12" si="7">F12-180</f>
+        <v>-154.04000000000002</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" ref="I12" si="8">ABS(C12/(E12-G12))</f>
+        <v>13.27531645569621</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>0.51</v>
+      </c>
+      <c r="C13" s="7">
+        <v>4.2149999999999999</v>
+      </c>
+      <c r="D13" s="7">
+        <v>116.1</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4.0869999999999997</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" ref="F13" si="9">D13-90</f>
+        <v>26.099999999999994</v>
+      </c>
+      <c r="G13" s="7">
+        <v>4.41</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" ref="H13" si="10">F13-180</f>
+        <v>-153.9</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" ref="I13" si="11">ABS(C13/(E13-G13))</f>
+        <v>13.049535603715153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50132EB3-244B-48AB-9E1D-E19B9F4F663D}">
+  <dimension ref="B3:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>6.2046860195077741E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16">
+        <v>2.7443</v>
+      </c>
+      <c r="D5" s="16">
+        <v>4.3710000000000004</v>
+      </c>
+      <c r="E5" s="16">
+        <f>(D5^2-C5^2)/(D5^2+C5^2)</f>
+        <v>0.43452848326097471</v>
+      </c>
+      <c r="I5">
+        <v>23</v>
+      </c>
+      <c r="J5">
+        <v>4.7388632927831797E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>0.12</v>
+      </c>
+      <c r="C6" s="16">
+        <v>3.7031000000000001</v>
+      </c>
+      <c r="D6" s="16">
+        <v>4.4863</v>
+      </c>
+      <c r="E6" s="16">
+        <f>(D6^2-C6^2)/(D6^2+C6^2)</f>
+        <v>0.18953808858885973</v>
+      </c>
+      <c r="I6">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <v>6.204939095583497E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>0.24</v>
+      </c>
+      <c r="C7" s="16">
+        <v>3.7877000000000001</v>
+      </c>
+      <c r="D7" s="16">
+        <v>4.3944000000000001</v>
+      </c>
+      <c r="E7" s="16">
+        <f>(D7^2-C7^2)/(D7^2+C7^2)</f>
+        <v>0.14748841946755545</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>0.36</v>
+      </c>
+      <c r="C8" s="16">
+        <v>3.8246000000000002</v>
+      </c>
+      <c r="D8" s="16">
+        <v>4.3314000000000004</v>
+      </c>
+      <c r="E8" s="16">
+        <f>(D8^2-C8^2)/(D8^2+C8^2)</f>
+        <v>0.12379859890296571</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>0.48</v>
+      </c>
+      <c r="C9" s="16">
+        <v>3.8534000000000002</v>
+      </c>
+      <c r="D9" s="16">
+        <v>4.2450000000000001</v>
+      </c>
+      <c r="E9" s="16">
+        <f>(D9^2-C9^2)/(D9^2+C9^2)</f>
+        <v>9.6484857697771917E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="16">
+        <v>3.8498000000000001</v>
+      </c>
+      <c r="D10" s="16">
+        <v>4.2008999999999999</v>
+      </c>
+      <c r="E10" s="16">
+        <f>(D10^2-C10^2)/(D10^2+C10^2)</f>
+        <v>8.7056653521683208E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="19">
+        <v>0.84</v>
+      </c>
+      <c r="C11" s="19">
+        <v>3.7696999999999998</v>
+      </c>
+      <c r="D11" s="19">
+        <v>4.056</v>
+      </c>
+      <c r="E11" s="19">
+        <f>(D11^2-C11^2)/(D11^2+C11^2)</f>
+        <v>7.3071372302971782E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="19"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
+        <v>0.84</v>
+      </c>
+      <c r="C16" s="16">
+        <v>3.7858999999999998</v>
+      </c>
+      <c r="D16" s="16">
+        <v>4.0956000000000001</v>
+      </c>
+      <c r="E16" s="17">
+        <f>(D16^2-C16^2)/(D16^2+C16^2)</f>
+        <v>7.8467941715857192E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="C17" s="16">
+        <v>3.8641999999999999</v>
+      </c>
+      <c r="D17" s="16">
+        <v>4.0811999999999999</v>
+      </c>
+      <c r="E17" s="17">
+        <f>(D17^2-C17^2)/(D17^2+C17^2)</f>
+        <v>5.4582087148377638E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
+        <v>1.08</v>
+      </c>
+      <c r="C18" s="16">
+        <v>3.9317000000000002</v>
+      </c>
+      <c r="D18" s="16">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="E18" s="17">
+        <f>(D18^2-C18^2)/(D18^2+C18^2)</f>
+        <v>4.4322069159820225E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="C19" s="16">
+        <v>3.9037999999999999</v>
+      </c>
+      <c r="D19" s="16">
+        <v>4.1505000000000001</v>
+      </c>
+      <c r="E19" s="17">
+        <f>(D19^2-C19^2)/(D19^2+C19^2)</f>
+        <v>6.1201785327050819E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
+        <v>1.03</v>
+      </c>
+      <c r="C20" s="16">
+        <v>3.9037999999999999</v>
+      </c>
+      <c r="D20" s="16">
+        <v>4.1505000000000001</v>
+      </c>
+      <c r="E20" s="17">
+        <f>(D20^2-C20^2)/(D20^2+C20^2)</f>
+        <v>6.1201785327050819E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resonator Syn - Initial Sweep (optimal Bridge=0.28)
</commit_message>
<xml_diff>
--- a/Fall 2023/Microwave Engineering/Project/Data.xlsx
+++ b/Fall 2023/Microwave Engineering/Project/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Fall 2023\Microwave Engineering\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youss\OneDrive\Documents\UCF\Fall 2023\Microwave Engineering\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DBF999-E5DF-4CE8-9253-6DCCA6C8C4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9B02F7-0B08-4C36-89ED-AB296655E03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>g</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Gap=0.42 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ======================= ATTEMPT 2 ========================</t>
+  </si>
+  <si>
+    <t>Flatness</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -266,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -279,9 +288,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -294,19 +302,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -314,56 +322,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -521,13 +479,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -541,6 +492,63 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3578,16 +3586,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{55FEDA29-AB2B-4C70-9B9B-75AB59D53983}" name="Table3" displayName="Table3" ref="B4:E12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{55FEDA29-AB2B-4C70-9B9B-75AB59D53983}" name="Table3" displayName="Table3" ref="B4:E12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B4:E12" xr:uid="{55FEDA29-AB2B-4C70-9B9B-75AB59D53983}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E11">
     <sortCondition ref="B4:B11"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F3E3B381-05AC-45A9-93A3-F0AB3D687519}" name="Spacing" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{7B3BD53E-1547-43C1-B438-211461B91917}" name="fm" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{3365EFB3-39BC-43B8-9F1A-AE6C8980A1F9}" name="fe" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3B3FEAE3-E71D-4113-B448-E8C1D7A50362}" name="kij" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{F3E3B381-05AC-45A9-93A3-F0AB3D687519}" name="Spacing" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{7B3BD53E-1547-43C1-B438-211461B91917}" name="fm" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{3365EFB3-39BC-43B8-9F1A-AE6C8980A1F9}" name="fe" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{3B3FEAE3-E71D-4113-B448-E8C1D7A50362}" name="kij" dataDxfId="0">
       <calculatedColumnFormula>(D5^2-C5^2)/(D5^2+C5^2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4685,10 +4693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBBA627-5AD6-4DBF-B35D-AA71A4FC1916}">
-  <dimension ref="B2:E28"/>
+  <dimension ref="B2:P83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="N84" sqref="N84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5017,6 +5025,178 @@
       </c>
       <c r="D28">
         <v>3.6015999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" t="s">
+        <v>38</v>
+      </c>
+      <c r="J77" t="s">
+        <v>31</v>
+      </c>
+      <c r="K77" t="s">
+        <v>32</v>
+      </c>
+      <c r="L77" t="s">
+        <v>19</v>
+      </c>
+      <c r="N77" t="s">
+        <v>31</v>
+      </c>
+      <c r="O77" t="s">
+        <v>32</v>
+      </c>
+      <c r="P77" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>0.2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>39</v>
+      </c>
+      <c r="J78">
+        <v>0.22</v>
+      </c>
+      <c r="K78">
+        <v>0.3</v>
+      </c>
+      <c r="L78">
+        <v>4.0859049207672999</v>
+      </c>
+      <c r="N78">
+        <v>0.24</v>
+      </c>
+      <c r="O78">
+        <v>0.3</v>
+      </c>
+      <c r="P78">
+        <v>4.0859049207672999</v>
+      </c>
+    </row>
+    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>0.22</v>
+      </c>
+      <c r="J79">
+        <v>0.22</v>
+      </c>
+      <c r="K79">
+        <v>0.32</v>
+      </c>
+      <c r="L79">
+        <v>3.8590492076730998</v>
+      </c>
+      <c r="N79">
+        <v>0.24</v>
+      </c>
+      <c r="O79">
+        <v>0.32</v>
+      </c>
+      <c r="P79">
+        <v>3.8590492076730998</v>
+      </c>
+    </row>
+    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>0.24</v>
+      </c>
+      <c r="J80">
+        <v>0.22</v>
+      </c>
+      <c r="K80">
+        <v>0.34</v>
+      </c>
+      <c r="L80">
+        <v>3.8590492076730998</v>
+      </c>
+      <c r="N80">
+        <v>0.24</v>
+      </c>
+      <c r="O80">
+        <v>0.34</v>
+      </c>
+      <c r="P80">
+        <v>3.8590492076730998</v>
+      </c>
+    </row>
+    <row r="81" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>0.26</v>
+      </c>
+      <c r="J81">
+        <v>0.22</v>
+      </c>
+      <c r="K81">
+        <v>0.36</v>
+      </c>
+      <c r="L81">
+        <v>3.8990825688072999</v>
+      </c>
+      <c r="N81">
+        <v>0.24</v>
+      </c>
+      <c r="O81">
+        <v>0.36</v>
+      </c>
+      <c r="P81">
+        <v>3.8990825688072999</v>
+      </c>
+    </row>
+    <row r="82" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J82">
+        <v>0.22</v>
+      </c>
+      <c r="K82">
+        <v>0.38</v>
+      </c>
+      <c r="L82">
+        <v>3.7589658048374002</v>
+      </c>
+      <c r="N82">
+        <v>0.24</v>
+      </c>
+      <c r="O82">
+        <v>0.38</v>
+      </c>
+      <c r="P82">
+        <v>3.7589658048374002</v>
+      </c>
+    </row>
+    <row r="83" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>0.3</v>
+      </c>
+      <c r="J83">
+        <v>0.22</v>
+      </c>
+      <c r="K83">
+        <v>0.4</v>
+      </c>
+      <c r="L83">
+        <v>3.3619683069224</v>
+      </c>
+      <c r="N83">
+        <v>0.24</v>
+      </c>
+      <c r="O83">
+        <v>0.4</v>
+      </c>
+      <c r="P83">
+        <v>3.3619683069224</v>
       </c>
     </row>
   </sheetData>
@@ -5044,28 +5224,28 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5073,27 +5253,27 @@
       <c r="B5" s="6">
         <v>0</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>4.141</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>110.05</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>4.0439999999999996</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <f>D5-90</f>
         <v>20.049999999999997</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>4.2779999999999996</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <f>F5-180</f>
         <v>-159.94999999999999</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <f>ABS(C5/(E5-G5))</f>
         <v>17.696581196581199</v>
       </c>
@@ -5102,27 +5282,27 @@
       <c r="B6" s="6">
         <v>0.6</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>4.2110000000000003</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>117.11</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>4.0830000000000002</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <f t="shared" ref="F6:F10" si="0">D6-90</f>
         <v>27.11</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>4.4109999999999996</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <f t="shared" ref="H6:H10" si="1">F6-180</f>
         <v>-152.88999999999999</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <f t="shared" ref="I6:I10" si="2">ABS(C6/(E6-G6))</f>
         <v>12.838414634146366</v>
       </c>
@@ -5131,27 +5311,27 @@
       <c r="B7" s="6">
         <v>1.2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>4.202</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>123.37</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>4.0570000000000004</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>33.370000000000005</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>4.4509999999999996</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <f t="shared" si="1"/>
         <v>-146.63</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <f t="shared" si="2"/>
         <v>10.66497461928936</v>
       </c>
@@ -5160,27 +5340,27 @@
       <c r="B8" s="6">
         <v>1.6</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>4.157</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>127.23</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>4.0019999999999998</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>37.230000000000004</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>4.4509999999999996</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <f t="shared" si="1"/>
         <v>-142.76999999999998</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <f t="shared" si="2"/>
         <v>9.2583518930957709</v>
       </c>
@@ -5189,27 +5369,27 @@
       <c r="B9" s="6">
         <v>2.4</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>4.1479999999999997</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>129.68</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>3.9750000000000001</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>39.680000000000007</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>4.4909999999999997</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <f t="shared" si="1"/>
         <v>-140.32</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <f t="shared" si="2"/>
         <v>8.038759689922486</v>
       </c>
@@ -5218,27 +5398,27 @@
       <c r="B10" s="6">
         <v>3</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>4.1059999999999999</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>138.69999999999999</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>3.9489999999999998</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>48.699999999999989</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>4.4889999999999999</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <f t="shared" si="1"/>
         <v>-131.30000000000001</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <f t="shared" si="2"/>
         <v>7.6037037037037027</v>
       </c>
@@ -5247,27 +5427,27 @@
       <c r="B11" s="6">
         <v>0.5</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>4.17</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>116.13</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>4.0490000000000004</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <f t="shared" ref="F11" si="3">D11-90</f>
         <v>26.129999999999995</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <v>4.3540000000000001</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <f t="shared" ref="H11" si="4">F11-180</f>
         <v>-153.87</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <f t="shared" ref="I11" si="5">ABS(C11/(E11-G11))</f>
         <v>13.672131147540997</v>
       </c>
@@ -5276,27 +5456,27 @@
       <c r="B12" s="6">
         <v>0.52</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>4.1950000000000003</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>115.96</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>4.07</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <f t="shared" ref="F12" si="6">D12-90</f>
         <v>25.959999999999994</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>4.3860000000000001</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <f t="shared" ref="H12" si="7">F12-180</f>
         <v>-154.04000000000002</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <f t="shared" ref="I12" si="8">ABS(C12/(E12-G12))</f>
         <v>13.27531645569621</v>
       </c>
@@ -5305,27 +5485,27 @@
       <c r="B13" s="6">
         <v>0.51</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>4.2149999999999999</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>116.1</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>4.0869999999999997</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <f t="shared" ref="F13" si="9">D13-90</f>
         <v>26.099999999999994</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="5">
         <v>4.41</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <f t="shared" ref="H13" si="10">F13-180</f>
         <v>-153.9</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <f t="shared" ref="I13" si="11">ABS(C13/(E13-G13))</f>
         <v>13.049535603715153</v>
       </c>
@@ -5340,7 +5520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50132EB3-244B-48AB-9E1D-E19B9F4F663D}">
   <dimension ref="B3:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -5361,16 +5541,16 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>1</v>
       </c>
       <c r="I4">
@@ -5381,17 +5561,17 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>0</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>2.7443</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>4.3710000000000004</v>
       </c>
-      <c r="E5" s="16">
-        <f>(D5^2-C5^2)/(D5^2+C5^2)</f>
+      <c r="E5" s="15">
+        <f t="shared" ref="E5:E11" si="0">(D5^2-C5^2)/(D5^2+C5^2)</f>
         <v>0.43452848326097471</v>
       </c>
       <c r="I5">
@@ -5402,17 +5582,17 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>0.12</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>3.7031000000000001</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>4.4863</v>
       </c>
-      <c r="E6" s="16">
-        <f>(D6^2-C6^2)/(D6^2+C6^2)</f>
+      <c r="E6" s="15">
+        <f t="shared" si="0"/>
         <v>0.18953808858885973</v>
       </c>
       <c r="I6">
@@ -5423,85 +5603,85 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>0.24</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>3.7877000000000001</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>4.3944000000000001</v>
       </c>
-      <c r="E7" s="16">
-        <f>(D7^2-C7^2)/(D7^2+C7^2)</f>
+      <c r="E7" s="15">
+        <f t="shared" si="0"/>
         <v>0.14748841946755545</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>0.36</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>3.8246000000000002</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>4.3314000000000004</v>
       </c>
-      <c r="E8" s="16">
-        <f>(D8^2-C8^2)/(D8^2+C8^2)</f>
+      <c r="E8" s="15">
+        <f t="shared" si="0"/>
         <v>0.12379859890296571</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>0.48</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>3.8534000000000002</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>4.2450000000000001</v>
       </c>
-      <c r="E9" s="16">
-        <f>(D9^2-C9^2)/(D9^2+C9^2)</f>
+      <c r="E9" s="15">
+        <f t="shared" si="0"/>
         <v>9.6484857697771917E-2</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>0.6</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>3.8498000000000001</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>4.2008999999999999</v>
       </c>
-      <c r="E10" s="16">
-        <f>(D10^2-C10^2)/(D10^2+C10^2)</f>
+      <c r="E10" s="15">
+        <f t="shared" si="0"/>
         <v>8.7056653521683208E-2</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="19">
+      <c r="B11" s="18">
         <v>0.84</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="18">
         <v>3.7696999999999998</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>4.056</v>
       </c>
-      <c r="E11" s="19">
-        <f>(D11^2-C11^2)/(D11^2+C11^2)</f>
+      <c r="E11" s="18">
+        <f t="shared" si="0"/>
         <v>7.3071372302971782E-2</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -5509,90 +5689,90 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>0.84</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>3.7858999999999998</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <v>4.0956000000000001</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <f>(D16^2-C16^2)/(D16^2+C16^2)</f>
         <v>7.8467941715857192E-2</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>0.96</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="15">
         <v>3.8641999999999999</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <v>4.0811999999999999</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <f>(D17^2-C17^2)/(D17^2+C17^2)</f>
         <v>5.4582087148377638E-2</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>1.08</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="15">
         <v>3.9317000000000002</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="15">
         <v>4.1100000000000003</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <f>(D18^2-C18^2)/(D18^2+C18^2)</f>
         <v>4.4322069159820225E-2</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>0.91100000000000003</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <v>3.9037999999999999</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="15">
         <v>4.1505000000000001</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="16">
         <f>(D19^2-C19^2)/(D19^2+C19^2)</f>
         <v>6.1201785327050819E-2</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>1.03</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="15">
         <v>3.9037999999999999</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="15">
         <v>4.1505000000000001</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <f>(D20^2-C20^2)/(D20^2+C20^2)</f>
         <v>6.1201785327050819E-2</v>
       </c>

</xml_diff>

<commit_message>
Please don't break github limit
</commit_message>
<xml_diff>
--- a/Fall 2023/Microwave Engineering/Project/Data.xlsx
+++ b/Fall 2023/Microwave Engineering/Project/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youss\OneDrive\Documents\UCF\Fall 2023\Microwave Engineering\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Fall 2023\Microwave Engineering\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9B02F7-0B08-4C36-89ED-AB296655E03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344DB346-03D4-40A6-86EE-D64BE0C70AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4DE9F586-C63E-4A23-BE5D-90A8419AB28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +186,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -275,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -316,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1582,6 +1591,330 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'K Synthesis'!$H$23:$H$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66669999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'K Synthesis'!$I$23:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.24695132711618101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18629289135483407</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15566950753325648</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10473752693918446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5109591125322348E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0678019890091787E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9762793155830322E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A0B-4805-9E38-71010025033D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="434008592"/>
+        <c:axId val="428492816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="434008592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="428492816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="428492816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="434008592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1702,6 +2035,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2722,6 +3095,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3538,6 +4427,42 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AC561FA-0ECA-7EAC-9AF6-88299E7357C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3902,8 +4827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C03D3BA-7F5A-483D-B888-8A7D711FA949}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F4"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4201,7 +5126,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>0.81279999999999997</v>
+        <v>0.78739999999999999</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -4277,8 +5202,8 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <f>(B13+1)/2 + (B13-1)*(1/SQRT(1+12*B14/B15))/2</f>
-        <v>2.7769535524233229</v>
+        <f>(B13+1)/2 + (B13-1)/(2*SQRT(1+12*B14/B15))</f>
+        <v>2.783715190080907</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4287,7 +5212,7 @@
       </c>
       <c r="B17">
         <f>B12/(B2*10^9*SQRT(B16))*1000</f>
-        <v>49.972824213095642</v>
+        <v>49.912095376812211</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -4300,7 +5225,7 @@
       </c>
       <c r="B18">
         <f>B17/2</f>
-        <v>24.986412106547821</v>
+        <v>24.956047688406105</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -4695,8 +5620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBBA627-5AD6-4DBF-B35D-AA71A4FC1916}">
   <dimension ref="B2:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="N84" sqref="N84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,6 +5950,27 @@
       </c>
       <c r="D28">
         <v>3.6015999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0.45350000000000001</v>
+      </c>
+      <c r="D39">
+        <v>3.5550000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>0.45319999999999999</v>
+      </c>
+      <c r="D40">
+        <v>3.6514000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>0.45334999999999998</v>
       </c>
     </row>
     <row r="76" spans="3:16" x14ac:dyDescent="0.25">
@@ -5209,8 +6155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257E1EC6-69F7-487F-B9CB-70A63808C60E}">
   <dimension ref="B3:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5251,89 +6197,89 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="C5" s="5">
-        <v>4.141</v>
+        <v>6.95</v>
       </c>
       <c r="D5" s="5">
-        <v>110.05</v>
+        <v>-80.69</v>
       </c>
       <c r="E5" s="5">
-        <v>4.0439999999999996</v>
+        <v>6.62</v>
       </c>
       <c r="F5" s="5">
         <f>D5-90</f>
-        <v>20.049999999999997</v>
+        <v>-170.69</v>
       </c>
       <c r="G5" s="5">
-        <v>4.2779999999999996</v>
+        <v>7.29</v>
       </c>
       <c r="H5" s="5">
-        <f>F5-180</f>
-        <v>-159.94999999999999</v>
+        <f>D5+90</f>
+        <v>9.3100000000000023</v>
       </c>
       <c r="I5" s="7">
         <f>ABS(C5/(E5-G5))</f>
-        <v>17.696581196581199</v>
+        <v>10.37313432835821</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
-        <v>0.6</v>
+        <v>-0.4</v>
       </c>
       <c r="C6" s="5">
-        <v>4.2110000000000003</v>
+        <v>6.9</v>
       </c>
       <c r="D6" s="5">
-        <v>117.11</v>
+        <v>-82.36</v>
       </c>
       <c r="E6" s="5">
-        <v>4.0830000000000002</v>
+        <v>6.56</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" ref="F6:F10" si="0">D6-90</f>
-        <v>27.11</v>
+        <v>-172.36</v>
       </c>
       <c r="G6" s="5">
-        <v>4.4109999999999996</v>
+        <v>7.26</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" ref="H6:H10" si="1">F6-180</f>
-        <v>-152.88999999999999</v>
+        <f t="shared" ref="H6:H13" si="1">D6+90</f>
+        <v>7.6400000000000006</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" ref="I6:I10" si="2">ABS(C6/(E6-G6))</f>
-        <v>12.838414634146366</v>
+        <v>9.8571428571428559</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
-        <v>1.2</v>
+        <v>0.66666665999999997</v>
       </c>
       <c r="C7" s="5">
-        <v>4.202</v>
+        <v>3.63</v>
       </c>
       <c r="D7" s="5">
-        <v>123.37</v>
+        <v>165.41</v>
       </c>
       <c r="E7" s="5">
-        <v>4.0570000000000004</v>
+        <v>3.4380000000000002</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>33.370000000000005</v>
+        <v>75.41</v>
       </c>
       <c r="G7" s="5">
-        <v>4.4509999999999996</v>
+        <v>3.8119999999999998</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="1"/>
-        <v>-146.63</v>
+        <v>255.41</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="2"/>
-        <v>10.66497461928936</v>
+        <v>9.7058823529411846</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -5358,7 +6304,7 @@
       </c>
       <c r="H8" s="5">
         <f t="shared" si="1"/>
-        <v>-142.76999999999998</v>
+        <v>217.23000000000002</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="2"/>
@@ -5387,7 +6333,7 @@
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
-        <v>-140.32</v>
+        <v>219.68</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="2"/>
@@ -5416,7 +6362,7 @@
       </c>
       <c r="H10" s="5">
         <f t="shared" si="1"/>
-        <v>-131.30000000000001</v>
+        <v>228.7</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="2"/>
@@ -5444,11 +6390,11 @@
         <v>4.3540000000000001</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" ref="H11" si="4">F11-180</f>
-        <v>-153.87</v>
+        <f t="shared" si="1"/>
+        <v>206.13</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" ref="I11" si="5">ABS(C11/(E11-G11))</f>
+        <f t="shared" ref="I11" si="4">ABS(C11/(E11-G11))</f>
         <v>13.672131147540997</v>
       </c>
     </row>
@@ -5466,18 +6412,18 @@
         <v>4.07</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" ref="F12" si="6">D12-90</f>
+        <f t="shared" ref="F12" si="5">D12-90</f>
         <v>25.959999999999994</v>
       </c>
       <c r="G12" s="5">
         <v>4.3860000000000001</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" ref="H12" si="7">F12-180</f>
-        <v>-154.04000000000002</v>
+        <f t="shared" si="1"/>
+        <v>205.95999999999998</v>
       </c>
       <c r="I12" s="7">
-        <f t="shared" ref="I12" si="8">ABS(C12/(E12-G12))</f>
+        <f t="shared" ref="I12" si="6">ABS(C12/(E12-G12))</f>
         <v>13.27531645569621</v>
       </c>
     </row>
@@ -5486,28 +6432,28 @@
         <v>0.51</v>
       </c>
       <c r="C13" s="5">
-        <v>4.2149999999999999</v>
+        <v>3.8580000000000001</v>
       </c>
       <c r="D13" s="5">
-        <v>116.1</v>
+        <v>161.29</v>
       </c>
       <c r="E13" s="5">
-        <v>4.0869999999999997</v>
+        <v>3.8180000000000001</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" ref="F13" si="9">D13-90</f>
-        <v>26.099999999999994</v>
+        <f t="shared" ref="F13" si="7">D13-90</f>
+        <v>71.289999999999992</v>
       </c>
       <c r="G13" s="5">
-        <v>4.41</v>
+        <v>4.0629999999999997</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" ref="H13" si="10">F13-180</f>
-        <v>-153.9</v>
+        <f t="shared" si="1"/>
+        <v>251.29</v>
       </c>
       <c r="I13" s="7">
-        <f t="shared" ref="I13" si="11">ABS(C13/(E13-G13))</f>
-        <v>13.049535603715153</v>
+        <f t="shared" ref="I13" si="8">ABS(C13/(E13-G13))</f>
+        <v>15.746938775510227</v>
       </c>
     </row>
   </sheetData>
@@ -5518,15 +6464,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50132EB3-244B-48AB-9E1D-E19B9F4F663D}">
-  <dimension ref="B3:J20"/>
+  <dimension ref="B3:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="J5" sqref="J4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -5562,17 +6510,17 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="15">
-        <v>0</v>
+        <v>0.63181818000000001</v>
       </c>
       <c r="C5" s="15">
-        <v>2.7443</v>
+        <v>3.4594999999999998</v>
       </c>
       <c r="D5" s="15">
-        <v>4.3710000000000004</v>
+        <v>3.7376</v>
       </c>
       <c r="E5" s="15">
-        <f t="shared" ref="E5:E11" si="0">(D5^2-C5^2)/(D5^2+C5^2)</f>
-        <v>0.43452848326097471</v>
+        <f t="shared" ref="E5:E12" si="0">(D5^2-C5^2)/(D5^2+C5^2)</f>
+        <v>7.7165911227004946E-2</v>
       </c>
       <c r="I5">
         <v>23</v>
@@ -5583,17 +6531,17 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="15">
-        <v>0.12</v>
+        <v>0.70909090909000005</v>
       </c>
       <c r="C6" s="15">
-        <v>3.7031000000000001</v>
+        <v>3.4725000000000001</v>
       </c>
       <c r="D6" s="15">
-        <v>4.4863</v>
+        <v>3.7261000000000002</v>
       </c>
       <c r="E6" s="15">
         <f t="shared" si="0"/>
-        <v>0.18953808858885973</v>
+        <v>7.0370808306113183E-2</v>
       </c>
       <c r="I6">
         <v>34</v>
@@ -5604,84 +6552,93 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="15">
-        <v>0.24</v>
+        <v>0.78636362999999998</v>
       </c>
       <c r="C7" s="15">
-        <v>3.7877000000000001</v>
+        <v>3.4868999999999999</v>
       </c>
       <c r="D7" s="15">
-        <v>4.3944000000000001</v>
+        <v>3.7130999999999998</v>
       </c>
       <c r="E7" s="15">
         <f t="shared" si="0"/>
-        <v>0.14748841946755545</v>
+        <v>6.2771377547781296E-2</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="15">
-        <v>0.36</v>
+        <v>0.86386386386299996</v>
       </c>
       <c r="C8" s="15">
-        <v>3.8246000000000002</v>
+        <v>3.5028000000000001</v>
       </c>
       <c r="D8" s="15">
-        <v>4.3314000000000004</v>
+        <v>3.7059000000000002</v>
       </c>
       <c r="E8" s="15">
         <f t="shared" si="0"/>
-        <v>0.12379859890296571</v>
+        <v>5.6303885306661236E-2</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15">
-        <v>0.48</v>
+        <v>0.94090909089999997</v>
       </c>
       <c r="C9" s="15">
-        <v>3.8534000000000002</v>
+        <v>3.52</v>
       </c>
       <c r="D9" s="15">
-        <v>4.2450000000000001</v>
+        <v>3.7000999999999999</v>
       </c>
       <c r="E9" s="15">
         <f t="shared" si="0"/>
-        <v>9.6484857697771917E-2</v>
+        <v>4.9857483587811904E-2</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="15">
-        <v>0.6</v>
+        <v>1.018181818</v>
       </c>
       <c r="C10" s="15">
-        <v>3.8498000000000001</v>
+        <v>3.5345</v>
       </c>
       <c r="D10" s="15">
-        <v>4.2008999999999999</v>
+        <v>3.6958000000000002</v>
       </c>
       <c r="E10" s="15">
         <f t="shared" si="0"/>
-        <v>8.7056653521683208E-2</v>
+        <v>4.4595594389210402E-2</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="18">
-        <v>0.84</v>
+        <v>1.0954545449999999</v>
       </c>
       <c r="C11" s="18">
-        <v>3.7696999999999998</v>
+        <v>3.5430999999999999</v>
       </c>
       <c r="D11" s="18">
-        <v>4.056</v>
+        <v>3.6886000000000001</v>
       </c>
       <c r="E11" s="18">
         <f t="shared" si="0"/>
-        <v>7.3071372302971782E-2</v>
+        <v>4.022321855117935E-2</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="C12" s="15">
+        <v>3.5604</v>
+      </c>
+      <c r="D12" s="15">
+        <v>3.68</v>
+      </c>
+      <c r="E12" s="18">
+        <f t="shared" si="0"/>
+        <v>3.3027836871991748E-2</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -5717,7 +6674,7 @@
         <v>7.8467941715857192E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <v>0.96</v>
       </c>
@@ -5732,7 +6689,7 @@
         <v>5.4582087148377638E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
         <v>1.08</v>
       </c>
@@ -5747,7 +6704,7 @@
         <v>4.4322069159820225E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
         <v>0.91100000000000003</v>
       </c>
@@ -5762,7 +6719,7 @@
         <v>6.1201785327050819E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="14">
         <v>1.03</v>
       </c>
@@ -5775,6 +6732,116 @@
       <c r="E20" s="16">
         <f>(D20^2-C20^2)/(D20^2+C20^2)</f>
         <v>6.1201785327050819E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="I23">
+        <v>0.24695132711618101</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I24">
+        <v>0.18629289135483407</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="19">
+        <v>0.63181818000000001</v>
+      </c>
+      <c r="D25" s="19">
+        <v>7.7165911000000004E-2</v>
+      </c>
+      <c r="H25" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="I25">
+        <v>0.15566950753325648</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="19">
+        <v>0.70909090900000005</v>
+      </c>
+      <c r="D26" s="19">
+        <v>7.0370808000000007E-2</v>
+      </c>
+      <c r="H26" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="I26">
+        <v>0.10473752693918446</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="19">
+        <v>0.78636362999999998</v>
+      </c>
+      <c r="D27" s="19">
+        <v>6.2771378000000003E-2</v>
+      </c>
+      <c r="H27" s="14">
+        <v>0.5333</v>
+      </c>
+      <c r="I27">
+        <v>8.5109591125322348E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="19">
+        <v>0.86386386400000004</v>
+      </c>
+      <c r="D28" s="19">
+        <v>5.6303884999999998E-2</v>
+      </c>
+      <c r="H28" s="14">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="I28">
+        <v>7.0678019890091787E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="19">
+        <v>0.94090909099999998</v>
+      </c>
+      <c r="D29" s="19">
+        <v>4.9857484000000001E-2</v>
+      </c>
+      <c r="H29" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="I29">
+        <v>5.9762793155830322E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="19">
+        <v>1.018181818</v>
+      </c>
+      <c r="D30" s="19">
+        <v>4.4595594000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="19">
+        <v>1.0954545449999999</v>
+      </c>
+      <c r="D31" s="19">
+        <v>4.0223218999999998E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="D32" s="19">
+        <v>3.3027836999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>